<commit_message>
some organization, added some common ui elements, initial modal setup
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A142224-C9CA-45D7-9308-6338D89AC382}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6332251C-B226-4332-9C54-E55F5F4227AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="3120" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Key</t>
   </si>
@@ -38,6 +38,36 @@
   </si>
   <si>
     <t>Welcome!</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Food Prep</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>sound</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
   </si>
 </sst>
 </file>
@@ -370,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,6 +442,46 @@
         <v>50</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
rebuild lightmap of main scene, merge start and main scene, initial intro implement
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6332251C-B226-4332-9C54-E55F5F4227AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F4012B-A7AD-44E4-90B6-1307A663C3E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="3120" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Key</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>CLOSE</t>
+  </si>
+  <si>
+    <t>intro_1</t>
+  </si>
+  <si>
+    <t>intro 1</t>
+  </si>
+  <si>
+    <t>intro_2</t>
+  </si>
+  <si>
+    <t>intro 2</t>
   </si>
 </sst>
 </file>
@@ -400,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,6 +494,22 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
food products art assets, prep. food product data
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F4012B-A7AD-44E4-90B6-1307A663C3E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4490F3D-D68A-426A-AD41-DFBDDBB94240}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="3120" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6165" yWindow="3630" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Key</t>
   </si>
@@ -80,6 +80,102 @@
   </si>
   <si>
     <t>intro 2</t>
+  </si>
+  <si>
+    <t>food_beef</t>
+  </si>
+  <si>
+    <t>Beef</t>
+  </si>
+  <si>
+    <t>food_eggs</t>
+  </si>
+  <si>
+    <t>Eggs</t>
+  </si>
+  <si>
+    <t>food_fruits</t>
+  </si>
+  <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>food_lamb</t>
+  </si>
+  <si>
+    <t>Lamb</t>
+  </si>
+  <si>
+    <t>food_mayo</t>
+  </si>
+  <si>
+    <t>Mayonnaise</t>
+  </si>
+  <si>
+    <t>food_milk</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>food_pork</t>
+  </si>
+  <si>
+    <t>Pork</t>
+  </si>
+  <si>
+    <t>food_poultry</t>
+  </si>
+  <si>
+    <t>Poultry</t>
+  </si>
+  <si>
+    <t>food_rice_cooked</t>
+  </si>
+  <si>
+    <t>Rice (Cooked)</t>
+  </si>
+  <si>
+    <t>food_shellfish</t>
+  </si>
+  <si>
+    <t>Shellfish</t>
+  </si>
+  <si>
+    <t>food_vegetables_sliced</t>
+  </si>
+  <si>
+    <t>Vegetables (Sliced)</t>
+  </si>
+  <si>
+    <t>food_bread</t>
+  </si>
+  <si>
+    <t>Bread (Plain)</t>
+  </si>
+  <si>
+    <t>food_cannedGoods</t>
+  </si>
+  <si>
+    <t>Canned Goods</t>
+  </si>
+  <si>
+    <t>food_flour</t>
+  </si>
+  <si>
+    <t>Flour</t>
+  </si>
+  <si>
+    <t>Rice (Raw)</t>
+  </si>
+  <si>
+    <t>food_rice_raw</t>
+  </si>
+  <si>
+    <t>food_potato</t>
+  </si>
+  <si>
+    <t>Potatoes (Raw)</t>
   </si>
 </sst>
 </file>
@@ -412,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,6 +606,134 @@
         <v>19</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
initial TCS Food module, some gameflow tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4490F3D-D68A-426A-AD41-DFBDDBB94240}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56412B44-9C5A-4C50-AB89-F36C14A643D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6165" yWindow="3630" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2355" yWindow="2790" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Key</t>
   </si>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>Potatoes (Raw)</t>
+  </si>
+  <si>
+    <t>tcs_foods</t>
+  </si>
+  <si>
+    <t>TCS Foods\n(Time/Temperature Control for Safety)</t>
+  </si>
+  <si>
+    <t>non_tcs_foods</t>
+  </si>
+  <si>
+    <t>Non-TCS Foods</t>
   </si>
 </sst>
 </file>
@@ -508,9 +520,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -592,145 +604,161 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>49</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added TCS Food list modal
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9F2ED6-68FE-4BC4-9478-8D36D12EE8B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B02E0E-3E32-4CF3-B4C7-381FE5C822D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2355" yWindow="2790" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>Key</t>
   </si>
@@ -194,6 +194,108 @@
   </si>
   <si>
     <t>SCORE:</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_meats</t>
+  </si>
+  <si>
+    <t>Meats</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_meats_title</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_poultry_title</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_poultry</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_seafood_title</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_seafood</t>
+  </si>
+  <si>
+    <t>Seafood</t>
+  </si>
+  <si>
+    <t>Fish, Salmon, Tuna</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_bakery_title</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_bakery</t>
+  </si>
+  <si>
+    <t>Bakery Foods</t>
+  </si>
+  <si>
+    <t>Cream pastries\nCream/custard pies and tarts\nPudding - prepared</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_dairy_title</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_dairy</t>
+  </si>
+  <si>
+    <t>Dairy Foods</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_pasta_title</t>
+  </si>
+  <si>
+    <t>Pasta</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_pasta</t>
+  </si>
+  <si>
+    <t>Noodles - all kinds, cooked\nRice - cooked</t>
+  </si>
+  <si>
+    <t>Chicken - ground, roasted, barbequed, fried, nuggets, patties, strips\nCasseroles with chicken/turkey\nDressing\nGravy\nPrecooked, processed products\nTurkey – ground, roast\nSoups Stews</t>
+  </si>
+  <si>
+    <t>Bacon - in raw form\nBeef - ground, roasts, steak\nGravy\nGround meats - all\nHot Dogs\nLunch meat\nMeat casseroles\nPork - ground, ham, roasts\nProcessed meats - all\nSausage\nSoups Stews</t>
+  </si>
+  <si>
+    <t>Whipped butter/whipped margarine\nCheese - mozzarella, cottage, cream, Ricotta\nCream - real, sauce, white\nDairy whipped topping\nIce cream\nMilk</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_eggs_title</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_eggs</t>
+  </si>
+  <si>
+    <t>Egg casseroles\nEgg dishes\nDeviled eggs\nFried eggs\nHard-cooked eggs\nOmelets\nScrambled eggs</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_fruits_veg_title</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_fruits_veg</t>
+  </si>
+  <si>
+    <t>Fruits and Vegetables</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_misc_title</t>
+  </si>
+  <si>
+    <t>tcsFoodDesc_misc</t>
+  </si>
+  <si>
+    <t>Misc.</t>
+  </si>
+  <si>
+    <t>Salad dressings prepared from a mix</t>
+  </si>
+  <si>
+    <t>Dry beans - cooked\nPotatoes - baked, boiled mashed (fresh, instant), scalloped/augratin (fresh, dehydrated)\nCut/prepared fresh fruits and vegetables (including melons, tomatoes and salad greens)</t>
   </si>
 </sst>
 </file>
@@ -526,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,6 +878,150 @@
         <v>48</v>
       </c>
     </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
some wash produce content
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B02E0E-3E32-4CF3-B4C7-381FE5C822D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49DDB3C-D9CA-44A3-8508-34A2B4ECD2F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="2790" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4455" yWindow="3045" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
   <si>
     <t>Key</t>
   </si>
@@ -296,6 +296,60 @@
   </si>
   <si>
     <t>Dry beans - cooked\nPotatoes - baked, boiled mashed (fresh, instant), scalloped/augratin (fresh, dehydrated)\nCut/prepared fresh fruits and vegetables (including melons, tomatoes and salad greens)</t>
+  </si>
+  <si>
+    <t>washProduce_title</t>
+  </si>
+  <si>
+    <t>Washing Produce</t>
+  </si>
+  <si>
+    <t>washProduce_item_1</t>
+  </si>
+  <si>
+    <t>washProduce_item_2</t>
+  </si>
+  <si>
+    <t>washProduce_item_3</t>
+  </si>
+  <si>
+    <t>washProduce_item_4</t>
+  </si>
+  <si>
+    <t>washProduce_item_5</t>
+  </si>
+  <si>
+    <t>washProduce_item_6</t>
+  </si>
+  <si>
+    <t>washProduce_item_7</t>
+  </si>
+  <si>
+    <t>Wash your hands for 20 seconds with warm water and soap before and after preparing fresh produce.</t>
+  </si>
+  <si>
+    <t>If damage or bruising occurs before eating or handling, cut away the damaged or bruised areas before preparing or eating.</t>
+  </si>
+  <si>
+    <t>Rinse produce BEFORE you peel it, so dirt and bacteria aren’t transferred from the knife onto the fruit or vegetable.</t>
+  </si>
+  <si>
+    <t>Gently rub produce while holding under plain running water. There’s no need to use soap or a produce wash.</t>
+  </si>
+  <si>
+    <t>Use a clean vegetable brush to scrub firm produce, such as melons and cucumbers.</t>
+  </si>
+  <si>
+    <t>Dry produce with a clean cloth or paper towel to further reduce bacteria that may be present.</t>
+  </si>
+  <si>
+    <t>Remove the outermost leaves of a head of lettuce or cabbage.</t>
+  </si>
+  <si>
+    <t>food_produce</t>
+  </si>
+  <si>
+    <t>Produce</t>
   </si>
 </sst>
 </file>
@@ -628,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,146 +934,242 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>62</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>63</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>64</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>67</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>68</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>71</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>72</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>74</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>76</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>81</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>82</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>84</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>85</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>87</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>88</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement thawing foods flow
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C40712-20F5-4E19-87CD-5E376D0A14D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A509378-25DD-4580-933E-2D7A93B683B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4455" yWindow="3045" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
   <si>
     <t>Key</t>
   </si>
@@ -356,6 +356,12 @@
   </si>
   <si>
     <t>Press the faucet to begin.</t>
+  </si>
+  <si>
+    <t>thawing_timer</t>
+  </si>
+  <si>
+    <t>Thawing Time</t>
   </si>
 </sst>
 </file>
@@ -688,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,323 +826,320 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
-      </c>
-      <c r="C49">
-        <v>2.5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C50">
-        <v>4</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C51">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C52">
         <v>6</v>
@@ -1144,10 +1147,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C53">
         <v>6</v>
@@ -1155,10 +1158,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C54">
         <v>6</v>
@@ -1166,10 +1169,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C55">
         <v>6</v>
@@ -1177,12 +1180,23 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>100</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>107</v>
       </c>
-      <c r="C56">
+      <c r="C57">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
initial thermometer calibration setup
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A509378-25DD-4580-933E-2D7A93B683B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C8ACAC-624A-40F8-A1C1-AC3256F34A92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4455" yWindow="3045" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
   <si>
     <t>Key</t>
   </si>
@@ -362,6 +362,12 @@
   </si>
   <si>
     <t>Thawing Time</t>
+  </si>
+  <si>
+    <t>thermometer_calibration</t>
+  </si>
+  <si>
+    <t>Thermometer Calibration</t>
   </si>
 </sst>
 </file>
@@ -694,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,323 +840,320 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
-      </c>
-      <c r="C50">
-        <v>2.5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C51">
-        <v>4</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C52">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C53">
         <v>6</v>
@@ -1158,10 +1161,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C54">
         <v>6</v>
@@ -1169,10 +1172,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C55">
         <v>6</v>
@@ -1180,10 +1183,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C56">
         <v>6</v>
@@ -1191,12 +1194,23 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>100</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>107</v>
       </c>
-      <c r="C57">
+      <c r="C58">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
thermometer calibrate functionalities and ui setup
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C8ACAC-624A-40F8-A1C1-AC3256F34A92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F6061B-2313-4860-8BF0-1CD4C541D228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4455" yWindow="3045" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
   <si>
     <t>Key</t>
   </si>
@@ -368,6 +368,24 @@
   </si>
   <si>
     <t>Thermometer Calibration</t>
+  </si>
+  <si>
+    <t>confirm</t>
+  </si>
+  <si>
+    <t>CONFIRM</t>
+  </si>
+  <si>
+    <t>thermometer_calibration_result</t>
+  </si>
+  <si>
+    <t>Thermometer Calibration Result</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>Target</t>
   </si>
 </sst>
 </file>
@@ -700,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,409 +802,400 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>93</v>
-      </c>
-      <c r="C51">
-        <v>2.5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52">
-        <v>4</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53">
-        <v>6</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C54">
-        <v>6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B55" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C55">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C56">
         <v>6</v>
@@ -1194,10 +1203,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C57">
         <v>6</v>
@@ -1205,12 +1214,45 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" t="s">
+        <v>104</v>
+      </c>
+      <c r="C58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>98</v>
+      </c>
+      <c r="B59" t="s">
+        <v>105</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" t="s">
+        <v>106</v>
+      </c>
+      <c r="C60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>100</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B61" t="s">
         <v>107</v>
       </c>
-      <c r="C58">
+      <c r="C61">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
thermometer adjust gameflow, some fixes
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F6061B-2313-4860-8BF0-1CD4C541D228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2683FBF-BDD3-49CA-8597-8CFE91E20CB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4455" yWindow="3045" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="132">
   <si>
     <t>Key</t>
   </si>
@@ -386,6 +386,36 @@
   </si>
   <si>
     <t>Target</t>
+  </si>
+  <si>
+    <t>thermometer_broken</t>
+  </si>
+  <si>
+    <t>Something is not right with this thermometer, should we proceed to use it?</t>
+  </si>
+  <si>
+    <t>Yeah, it's fine.</t>
+  </si>
+  <si>
+    <t>thermometer_broken0</t>
+  </si>
+  <si>
+    <t>thermometer_broken1</t>
+  </si>
+  <si>
+    <t>No, it's broken.</t>
+  </si>
+  <si>
+    <t>thermometer_broken_correct</t>
+  </si>
+  <si>
+    <t>thermometer_broken_wrong</t>
+  </si>
+  <si>
+    <t>Wrong! The arrow wasn't moving at all when the thermometer was dipped into the glass of ice.</t>
+  </si>
+  <si>
+    <t>That's right, the arrow wasn't moving at all when the thermometer was dipped into the glass of ice. Good call!</t>
   </si>
 </sst>
 </file>
@@ -718,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,6 +1286,55 @@
         <v>5</v>
       </c>
     </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
added hud score, some bug fix
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2683FBF-BDD3-49CA-8597-8CFE91E20CB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C0A500-E971-4190-BE59-82FE780DBC20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4455" yWindow="3045" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="134">
   <si>
     <t>Key</t>
   </si>
@@ -412,10 +412,16 @@
     <t>thermometer_broken_wrong</t>
   </si>
   <si>
-    <t>Wrong! The arrow wasn't moving at all when the thermometer was dipped into the glass of ice.</t>
-  </si>
-  <si>
-    <t>That's right, the arrow wasn't moving at all when the thermometer was dipped into the glass of ice. Good call!</t>
+    <t>score_total</t>
+  </si>
+  <si>
+    <t>TOTAL SCORE:</t>
+  </si>
+  <si>
+    <t>That's right, the thermometer's arrow didn't move when it was dipped into the glass. Good call!</t>
+  </si>
+  <si>
+    <t>Wrong! The thermometer's arrow didn't move when it was dipped into the glass.</t>
   </si>
 </sst>
 </file>
@@ -748,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,363 +886,360 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B45" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B48" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B51" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s">
-        <v>93</v>
-      </c>
-      <c r="C54">
-        <v>2.5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B55" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C55">
-        <v>4</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C56">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C57">
         <v>6</v>
@@ -1244,10 +1247,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C58">
         <v>6</v>
@@ -1255,10 +1258,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C59">
         <v>6</v>
@@ -1266,10 +1269,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C60">
         <v>6</v>
@@ -1277,62 +1280,73 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C62">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C63">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C64">
         <v>1.5</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>128</v>
       </c>
-      <c r="B65" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="B66" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>129</v>
       </c>
-      <c r="B66" t="s">
-        <v>130</v>
+      <c r="B67" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
danger zone game flow, some fixes
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C0A500-E971-4190-BE59-82FE780DBC20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257A4329-CF00-4E6A-AE5E-2E81CD7D2E2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4455" yWindow="3045" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
   <si>
     <t>Key</t>
   </si>
@@ -422,6 +422,30 @@
   </si>
   <si>
     <t>Wrong! The thermometer's arrow didn't move when it was dipped into the glass.</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia1</t>
+  </si>
+  <si>
+    <t>food_beefStew</t>
+  </si>
+  <si>
+    <t>Beef Stew</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia10</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia11</t>
+  </si>
+  <si>
+    <t>A pot of beef stew has been placed in an ice-water bath to cool. After constant stirring, three hours have passed, and the temperature reads 70° F. Is the beef stew ready to be placed into the cooler?</t>
+  </si>
+  <si>
+    <t>Yes, the stew has reached the proper temperature of 70° F, it should be ready to be placed in the cooler.</t>
+  </si>
+  <si>
+    <t>No, the temperature didn't reach 70° F before two hours, it should be thrown out.</t>
   </si>
 </sst>
 </file>
@@ -754,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,187 +1094,184 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>135</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B48" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B53" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B55" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55">
-        <v>2.5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B56" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C56">
-        <v>4</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C57">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C58">
         <v>6</v>
@@ -1258,10 +1279,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B59" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C59">
         <v>6</v>
@@ -1269,10 +1290,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C60">
         <v>6</v>
@@ -1280,10 +1301,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C61">
         <v>6</v>
@@ -1291,43 +1312,43 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C62">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="B63" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C64">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C65">
         <v>1.5</v>
@@ -1335,18 +1356,53 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>127</v>
+      </c>
+      <c r="C66">
+        <v>1.5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>128</v>
+      </c>
+      <c r="B67" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>129</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>137</v>
+      </c>
+      <c r="B70" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>138</v>
+      </c>
+      <c r="B71" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
danger zone gameplay content
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257A4329-CF00-4E6A-AE5E-2E81CD7D2E2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D1430A-E405-4787-81CB-FE2D3689B9EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4455" yWindow="3045" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="177">
   <si>
     <t>Key</t>
   </si>
@@ -446,6 +446,111 @@
   </si>
   <si>
     <t>No, the temperature didn't reach 70° F before two hours, it should be thrown out.</t>
+  </si>
+  <si>
+    <t>food_bbqPork</t>
+  </si>
+  <si>
+    <t>Barbeque Pork</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia2</t>
+  </si>
+  <si>
+    <t>A tray of barbeque pork has been placed in the oven to be reheated. After 30 minutes, a server checks the internal temperature for 15 seconds. It reads 165° F.</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia20</t>
+  </si>
+  <si>
+    <t>The temperature looks good, it is ready to be served.</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia21</t>
+  </si>
+  <si>
+    <t>It still needs to be heated, put it back in the oven, and wait for another 30 minutes.</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia22</t>
+  </si>
+  <si>
+    <t>It is not safe to be served, throw it out.</t>
+  </si>
+  <si>
+    <t>food_bbqChicken</t>
+  </si>
+  <si>
+    <t>Barbeque Chicken</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia3</t>
+  </si>
+  <si>
+    <t>A server has been sent to check on the temperature of a tray of barbeque chicken. After checking the internal temperature for 15 seconds, it reads 127° F. The tray has been out for at least an hour.</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia30</t>
+  </si>
+  <si>
+    <t>The tray needs to be heated up.</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia31</t>
+  </si>
+  <si>
+    <t>food_broccoliSalad</t>
+  </si>
+  <si>
+    <t>Broccoli Salad</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia4</t>
+  </si>
+  <si>
+    <t>The temperature looks good, leave it alone.</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia40</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia41</t>
+  </si>
+  <si>
+    <t>These shouldn't be served, replace it with a new batch.</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia42</t>
+  </si>
+  <si>
+    <t>It's too cold, they need to be heated up in a microwave.</t>
+  </si>
+  <si>
+    <t>Several broccoli salad trays being served have been out for more than an hour. A server decided to check the temperature of each tray. They all read 40° F.</t>
+  </si>
+  <si>
+    <t>food_yogurtBar</t>
+  </si>
+  <si>
+    <t>Yogurt Bar</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia5</t>
+  </si>
+  <si>
+    <t>A server was requested to check on the yogurt batch being served at the yogurt bar. After checking the temperature, it reads 53° F. Looking at the time it was brought out, it's been several hours.</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia50</t>
+  </si>
+  <si>
+    <t>This batch needs to be replaced.</t>
+  </si>
+  <si>
+    <t>dangerZoneTrivia51</t>
+  </si>
+  <si>
+    <t>The temperature is fine, leave it as is.</t>
   </si>
 </sst>
 </file>
@@ -778,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,220 +1207,208 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>159</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>169</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B48" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B52" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B53" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>93</v>
-      </c>
-      <c r="C56">
-        <v>2.5</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B57" t="s">
-        <v>101</v>
-      </c>
-      <c r="C57">
-        <v>4</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B58" t="s">
-        <v>102</v>
-      </c>
-      <c r="C58">
-        <v>6</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>103</v>
-      </c>
-      <c r="C59">
-        <v>6</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B60" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C60">
-        <v>6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B61" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C61">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B62" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C62">
         <v>6</v>
@@ -1323,86 +1416,242 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="B64" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="C64">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="B65" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="C65">
-        <v>1.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C66">
-        <v>1.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
+        <v>107</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B68" t="s">
-        <v>133</v>
+        <v>123</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>139</v>
+        <v>124</v>
+      </c>
+      <c r="C69">
+        <v>1.5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B70" t="s">
-        <v>141</v>
+        <v>127</v>
+      </c>
+      <c r="C70">
+        <v>1.5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>128</v>
+      </c>
+      <c r="B71" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>129</v>
+      </c>
+      <c r="B72" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>134</v>
+      </c>
+      <c r="B73" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>137</v>
+      </c>
+      <c r="B74" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>138</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B75" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>144</v>
+      </c>
+      <c r="B76" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>146</v>
+      </c>
+      <c r="B77" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>148</v>
+      </c>
+      <c r="B78" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>150</v>
+      </c>
+      <c r="B79" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>154</v>
+      </c>
+      <c r="B80" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>156</v>
+      </c>
+      <c r="B81" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>158</v>
+      </c>
+      <c r="B82" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>161</v>
+      </c>
+      <c r="B83" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>163</v>
+      </c>
+      <c r="B84" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>164</v>
+      </c>
+      <c r="B85" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>166</v>
+      </c>
+      <c r="B86" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
thawing explanation and details
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF456FC3-64DD-498A-B6D5-9E8827797826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9946EA3D-91CA-488E-BC5B-94D1F7AE3903}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="3120" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2265" yWindow="2385" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="261">
   <si>
     <t>Key</t>
   </si>
@@ -634,13 +634,175 @@
     <t>sanitaryEnd_1</t>
   </si>
   <si>
-    <t>Alright, we are good to go! Let's go ahead and start prepping the food we need for the day.</t>
-  </si>
-  <si>
     <t>Alright, looks like the other servers have arrived.</t>
   </si>
   <si>
     <t>They'll be heading out to their stations now.</t>
+  </si>
+  <si>
+    <t>Alright, we are good to go! Let's go ahead and start prepping for the day.</t>
+  </si>
+  <si>
+    <t>tcsIntro_1</t>
+  </si>
+  <si>
+    <t>First thing we need to do is determine which foods are potentially hazardous. The ones that allow pathogen growth.</t>
+  </si>
+  <si>
+    <t>tcsIntro_2</t>
+  </si>
+  <si>
+    <t>The best way to deal with these foods is through proper time management, and temperature control.</t>
+  </si>
+  <si>
+    <t>tcsIntro_3</t>
+  </si>
+  <si>
+    <t>This is known as Time and Temperature Control for Safety, or in short: TCS food.</t>
+  </si>
+  <si>
+    <t>tcsIntro_4</t>
+  </si>
+  <si>
+    <t>Most of these foods are easily identified through common sense. So, let’s see if you can identify which ones are TCS or non-TCS food.</t>
+  </si>
+  <si>
+    <t>tcsPost_1</t>
+  </si>
+  <si>
+    <t>Excellent! Now that that’s sorted out, let me show you a comprehensive list for TCS food.</t>
+  </si>
+  <si>
+    <t>produceIntro_1</t>
+  </si>
+  <si>
+    <t>Since the majority of foods already carry germs, steps must be taken to minimize the potential danger of these foods possess.</t>
+  </si>
+  <si>
+    <t>produceIntro_2</t>
+  </si>
+  <si>
+    <t>As such, all produce needs to be thoroughly washed to remove germs, and wash away insecticides.</t>
+  </si>
+  <si>
+    <t>produceIntro_3</t>
+  </si>
+  <si>
+    <t>Here are some useful tips for washing produce.</t>
+  </si>
+  <si>
+    <t>thawMethods_title</t>
+  </si>
+  <si>
+    <t>Thawing Methods</t>
+  </si>
+  <si>
+    <t>thawMethods_fridge_title</t>
+  </si>
+  <si>
+    <t>Refridgerator</t>
+  </si>
+  <si>
+    <t>thawMethods_fridge_desc</t>
+  </si>
+  <si>
+    <t>Thaw food in a refrigerator at 41° F (5° C) or lower to keep dangerous microorganisms from growing. Plan ahead when thawing large items such as turkeys - they can take several days to thaw.</t>
+  </si>
+  <si>
+    <t>thawMethods_water_title</t>
+  </si>
+  <si>
+    <t>thawMethods_water_desc</t>
+  </si>
+  <si>
+    <t>Running Water</t>
+  </si>
+  <si>
+    <t>Thaw food submerged under running water at a temperature of 70° F (21° C) or lower. The water flow must be strong enough to wash food particles into the overflow drain.</t>
+  </si>
+  <si>
+    <t>thawMethods_microwave_title</t>
+  </si>
+  <si>
+    <t>thawMethods_microwave_desc</t>
+  </si>
+  <si>
+    <t>Microwave</t>
+  </si>
+  <si>
+    <t>You can safely thaw food in a microwave oven if the food will be cooked immediately. Large items such as roasts or turkeys may not thaw well in a microwave.</t>
+  </si>
+  <si>
+    <t>thawIntro_1</t>
+  </si>
+  <si>
+    <t>Now we will talk about proper thawing of food.</t>
+  </si>
+  <si>
+    <t>thawIntro_2</t>
+  </si>
+  <si>
+    <t>thawIntro_3</t>
+  </si>
+  <si>
+    <t>There are several ways to thaw food. Each method varies by how long it takes. So, plan accordingly!</t>
+  </si>
+  <si>
+    <t>Here are the three methods commonly used.</t>
+  </si>
+  <si>
+    <t>thawFaucet_1</t>
+  </si>
+  <si>
+    <t>thawFaucet_2</t>
+  </si>
+  <si>
+    <t>For this exercise, we will be using the running water method.</t>
+  </si>
+  <si>
+    <t>Let’s start by turning the faucet on.</t>
+  </si>
+  <si>
+    <t>thawMeat_1</t>
+  </si>
+  <si>
+    <t>Great, now grab the pack of meat and put it under the running water.</t>
+  </si>
+  <si>
+    <t>thawWait_1</t>
+  </si>
+  <si>
+    <t>Excellent! Now just wait till the meat has properly thawed…It should take about half an hour to an hour.</t>
+  </si>
+  <si>
+    <t>Alright, well this will obviously take a while, so let’s compress time to speed things up!</t>
+  </si>
+  <si>
+    <t>thawWait_2</t>
+  </si>
+  <si>
+    <t>thawEnd_1</t>
+  </si>
+  <si>
+    <t>Great! The meat has been properly thawed and is ready to be cooked.</t>
+  </si>
+  <si>
+    <t>thawEnd_2</t>
+  </si>
+  <si>
+    <t>Remember that once food has been thawed, it must be cooked right away! Don’t put any of them back in the freezer!</t>
+  </si>
+  <si>
+    <t>calibrateIntro_1</t>
+  </si>
+  <si>
+    <t>Let's now talk about properly calibrating a thermometer.</t>
+  </si>
+  <si>
+    <t>calibrateIntro_2</t>
+  </si>
+  <si>
+    <t>Before using a thermometer, make sure it is calibrated properly!</t>
   </si>
 </sst>
 </file>
@@ -976,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D104"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1784,7 +1946,7 @@
         <v>185</v>
       </c>
       <c r="B94" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1792,7 +1954,7 @@
         <v>200</v>
       </c>
       <c r="B95" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1864,7 +2026,241 @@
         <v>203</v>
       </c>
       <c r="B104" t="s">
-        <v>204</v>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>207</v>
+      </c>
+      <c r="B105" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>209</v>
+      </c>
+      <c r="B106" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>211</v>
+      </c>
+      <c r="B107" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>213</v>
+      </c>
+      <c r="B108" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>215</v>
+      </c>
+      <c r="B109" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>217</v>
+      </c>
+      <c r="B110" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>219</v>
+      </c>
+      <c r="B111" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>221</v>
+      </c>
+      <c r="B112" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>223</v>
+      </c>
+      <c r="B113" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>225</v>
+      </c>
+      <c r="B114" t="s">
+        <v>226</v>
+      </c>
+      <c r="C114">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>227</v>
+      </c>
+      <c r="B115" t="s">
+        <v>228</v>
+      </c>
+      <c r="C115">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>229</v>
+      </c>
+      <c r="B116" t="s">
+        <v>231</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>230</v>
+      </c>
+      <c r="B117" t="s">
+        <v>232</v>
+      </c>
+      <c r="C117">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>233</v>
+      </c>
+      <c r="B118" t="s">
+        <v>235</v>
+      </c>
+      <c r="C118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>234</v>
+      </c>
+      <c r="B119" t="s">
+        <v>236</v>
+      </c>
+      <c r="C119">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>237</v>
+      </c>
+      <c r="B120" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>239</v>
+      </c>
+      <c r="B121" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>240</v>
+      </c>
+      <c r="B122" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>243</v>
+      </c>
+      <c r="B123" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>244</v>
+      </c>
+      <c r="B124" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>247</v>
+      </c>
+      <c r="B125" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>249</v>
+      </c>
+      <c r="B126" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>252</v>
+      </c>
+      <c r="B127" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>253</v>
+      </c>
+      <c r="B128" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>255</v>
+      </c>
+      <c r="B129" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>257</v>
+      </c>
+      <c r="B130" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>259</v>
+      </c>
+      <c r="B131" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some adjustments, build test
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93020C95-AC9E-46EF-9CA0-1B048D99C697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2C5F44-9624-44EE-B33A-40036052F371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2265" yWindow="2385" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,18 +538,9 @@
     <t>The temperature is fine, leave it as is.</t>
   </si>
   <si>
-    <t>Hello! I’m here to talk to you about the various safety procedures involved in food preparation.</t>
-  </si>
-  <si>
-    <t>First off, let’s talk about personal hygiene!</t>
-  </si>
-  <si>
     <t>intro_3</t>
   </si>
   <si>
-    <t>One of the most important steps before handling food is washing your hands.</t>
-  </si>
-  <si>
     <t>intro_4</t>
   </si>
   <si>
@@ -583,9 +574,6 @@
     <t>sanitaryInteract0</t>
   </si>
   <si>
-    <t>She seems functional enough to get to work, she should be fine.</t>
-  </si>
-  <si>
     <t>sanitaryInteract1</t>
   </si>
   <si>
@@ -601,36 +589,18 @@
     <t>sanitaryInteractResult1</t>
   </si>
   <si>
-    <t>Wearing a face mask is not enough! She shouldn't be here today!</t>
-  </si>
-  <si>
     <t>sanitaryInteractResult2</t>
   </si>
   <si>
     <t>That's correct, any employee suffering from respiratory or intestinal illness should not work their scheduled shift.</t>
   </si>
   <si>
-    <t>Uh oh, she appears to be sick. What's the best course of action?</t>
-  </si>
-  <si>
     <t>sanitary_2</t>
   </si>
   <si>
-    <t>She should take her leave for the day.</t>
-  </si>
-  <si>
-    <t>No way! She needs to take her leave for the day!</t>
-  </si>
-  <si>
     <t>sanitaryEnd_1</t>
   </si>
   <si>
-    <t>Alright, looks like the other servers have arrived.</t>
-  </si>
-  <si>
-    <t>They'll be heading out to their stations now.</t>
-  </si>
-  <si>
     <t>Alright, we are good to go! Let's go ahead and start prepping for the day.</t>
   </si>
   <si>
@@ -953,6 +923,36 @@
   </si>
   <si>
     <t>&lt;size=60&gt;Food Prepper&lt;/size&gt;\nSafety First</t>
+  </si>
+  <si>
+    <t>Greetings! We’re here today to learn about safety in food preparations.</t>
+  </si>
+  <si>
+    <t>Before we begin, it’s important to learn about proper hygiene!</t>
+  </si>
+  <si>
+    <t>First off, washing your hands. If there’s one place in our body to find a thriving colony of pathogens, it’s our hands.</t>
+  </si>
+  <si>
+    <t>They’re pumped up and ready to go!</t>
+  </si>
+  <si>
+    <t>Look at that, the other servers have arrived.</t>
+  </si>
+  <si>
+    <t>Hm, looks like one of the servers appears to be sick. What’s the best course of action?</t>
+  </si>
+  <si>
+    <t>She seems functional enough to work, she should be fine.</t>
+  </si>
+  <si>
+    <t>She should take a sick leave.</t>
+  </si>
+  <si>
+    <t>No way! Not only will she potentially infect other servers, but the customers as well! She needs to take a sick leave.</t>
+  </si>
+  <si>
+    <t>Wearing a face mask is not enough! We do not want to take any risk when someone is sick. She needs to take a sick leave.</t>
   </si>
 </sst>
 </file>
@@ -1290,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,15 +1335,15 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="B4" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1388,10 +1388,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="B10" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,26 +1420,26 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="B14" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="B15" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="B16" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2080,7 +2080,7 @@
         <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>172</v>
+        <v>301</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2088,71 +2088,71 @@
         <v>16</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>173</v>
+        <v>302</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B94" t="s">
-        <v>175</v>
+        <v>303</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B95" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B96" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B97" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B98" t="s">
-        <v>201</v>
+        <v>305</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B99" t="s">
-        <v>202</v>
+        <v>304</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B100" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B101" t="s">
-        <v>196</v>
+        <v>306</v>
       </c>
       <c r="C101">
         <v>6</v>
@@ -2160,10 +2160,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B102" t="s">
-        <v>187</v>
+        <v>307</v>
       </c>
       <c r="C102">
         <v>5</v>
@@ -2171,10 +2171,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B103" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C103">
         <v>5</v>
@@ -2182,10 +2182,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B104" t="s">
-        <v>198</v>
+        <v>308</v>
       </c>
       <c r="C104">
         <v>5</v>
@@ -2193,114 +2193,114 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B105" t="s">
-        <v>199</v>
+        <v>309</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B106" t="s">
-        <v>193</v>
+        <v>310</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B107" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B108" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B109" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B110" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B111" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B112" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B113" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B114" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B115" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B116" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B117" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B118" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C118">
         <v>1.5</v>
@@ -2308,10 +2308,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B119" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C119">
         <v>8</v>
@@ -2319,10 +2319,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B120" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C120">
         <v>2</v>
@@ -2330,10 +2330,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B121" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="C121">
         <v>8</v>
@@ -2341,10 +2341,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B122" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -2352,10 +2352,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B123" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C123">
         <v>8</v>
@@ -2363,266 +2363,266 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B124" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B125" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B126" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B127" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B128" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B129" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B130" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B131" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B132" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="B133" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="B134" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B135" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B136" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B137" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B138" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B139" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B140" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B141" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B142" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="B143" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="B144" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B145" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="B147" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="B148" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="B149" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="B152" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="B154" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="B155" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="B156" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed thermometer buttons to -/+, updated language, now able to run web game again in editor
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2C5F44-9624-44EE-B33A-40036052F371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE431906-12B3-4EB2-94ED-328D47779A16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2265" yWindow="2385" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,9 +637,6 @@
     <t>produceIntro_1</t>
   </si>
   <si>
-    <t>Since the majority of foods already carry germs, steps must be taken to minimize the potential danger of these foods possess.</t>
-  </si>
-  <si>
     <t>produceIntro_2</t>
   </si>
   <si>
@@ -953,6 +950,9 @@
   </si>
   <si>
     <t>Wearing a face mask is not enough! We do not want to take any risk when someone is sick. She needs to take a sick leave.</t>
+  </si>
+  <si>
+    <t>Since the majority of foods already carry germs, steps must be taken to minimize the potential danger these foods possess.</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1291,7 @@
   <dimension ref="A1:D156"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,15 +1335,15 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B4" t="s">
         <v>298</v>
-      </c>
-      <c r="B4" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1388,10 +1388,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B10" t="s">
         <v>290</v>
-      </c>
-      <c r="B10" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,26 +1420,26 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" t="s">
         <v>292</v>
-      </c>
-      <c r="B14" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B15" t="s">
         <v>294</v>
-      </c>
-      <c r="B15" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>295</v>
+      </c>
+      <c r="B16" t="s">
         <v>296</v>
-      </c>
-      <c r="B16" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2080,7 +2080,7 @@
         <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
         <v>16</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2096,7 +2096,7 @@
         <v>172</v>
       </c>
       <c r="B94" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2128,7 +2128,7 @@
         <v>179</v>
       </c>
       <c r="B98" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2136,7 +2136,7 @@
         <v>191</v>
       </c>
       <c r="B99" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -2152,7 +2152,7 @@
         <v>182</v>
       </c>
       <c r="B101" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C101">
         <v>6</v>
@@ -2163,7 +2163,7 @@
         <v>183</v>
       </c>
       <c r="B102" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C102">
         <v>5</v>
@@ -2185,7 +2185,7 @@
         <v>186</v>
       </c>
       <c r="B104" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C104">
         <v>5</v>
@@ -2196,7 +2196,7 @@
         <v>187</v>
       </c>
       <c r="B105" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2204,7 +2204,7 @@
         <v>188</v>
       </c>
       <c r="B106" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2268,39 +2268,39 @@
         <v>204</v>
       </c>
       <c r="B114" t="s">
-        <v>205</v>
+        <v>310</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>205</v>
+      </c>
+      <c r="B115" t="s">
         <v>206</v>
-      </c>
-      <c r="B115" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>207</v>
+      </c>
+      <c r="B116" t="s">
         <v>208</v>
-      </c>
-      <c r="B116" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>209</v>
+      </c>
+      <c r="B117" t="s">
         <v>210</v>
-      </c>
-      <c r="B117" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>211</v>
+      </c>
+      <c r="B118" t="s">
         <v>212</v>
-      </c>
-      <c r="B118" t="s">
-        <v>213</v>
       </c>
       <c r="C118">
         <v>1.5</v>
@@ -2308,10 +2308,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>213</v>
+      </c>
+      <c r="B119" t="s">
         <v>214</v>
-      </c>
-      <c r="B119" t="s">
-        <v>215</v>
       </c>
       <c r="C119">
         <v>8</v>
@@ -2319,10 +2319,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B120" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C120">
         <v>2</v>
@@ -2330,10 +2330,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B121" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C121">
         <v>8</v>
@@ -2341,10 +2341,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B122" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -2352,10 +2352,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B123" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C123">
         <v>8</v>
@@ -2363,266 +2363,266 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>223</v>
+      </c>
+      <c r="B124" t="s">
         <v>224</v>
-      </c>
-      <c r="B124" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B125" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B126" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B127" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B128" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>233</v>
+      </c>
+      <c r="B129" t="s">
         <v>234</v>
-      </c>
-      <c r="B129" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>235</v>
+      </c>
+      <c r="B130" t="s">
         <v>236</v>
-      </c>
-      <c r="B130" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B131" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>239</v>
+      </c>
+      <c r="B132" t="s">
         <v>240</v>
-      </c>
-      <c r="B132" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>241</v>
+      </c>
+      <c r="B133" t="s">
         <v>242</v>
-      </c>
-      <c r="B133" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B134" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B135" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>247</v>
+      </c>
+      <c r="B136" t="s">
         <v>248</v>
-      </c>
-      <c r="B136" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B137" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>250</v>
+      </c>
+      <c r="B138" t="s">
         <v>251</v>
-      </c>
-      <c r="B138" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>253</v>
+      </c>
+      <c r="B139" t="s">
         <v>254</v>
-      </c>
-      <c r="B139" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B140" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>256</v>
+      </c>
+      <c r="B141" t="s">
         <v>257</v>
-      </c>
-      <c r="B141" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>259</v>
+      </c>
+      <c r="B142" t="s">
         <v>260</v>
-      </c>
-      <c r="B142" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B143" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B144" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B145" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>267</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B147" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B148" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B149" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B152" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B154" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B155" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B156" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
show extra description after answering a trivia.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE431906-12B3-4EB2-94ED-328D47779A16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02213018-9E3E-4DAB-B99F-0B182A07F4AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="2385" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2265" yWindow="2385" windowWidth="22755" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="321">
   <si>
     <t>Key</t>
   </si>
@@ -523,9 +523,6 @@
     <t>dangerZoneTrivia5</t>
   </si>
   <si>
-    <t>A server was requested to check on the yogurt batch being served at the yogurt bar. After checking the temperature, it reads 53° F. Looking at the time it was brought out, it's been several hours.</t>
-  </si>
-  <si>
     <t>dangerZoneTrivia50</t>
   </si>
   <si>
@@ -953,6 +950,39 @@
   </si>
   <si>
     <t>Since the majority of foods already carry germs, steps must be taken to minimize the potential danger these foods possess.</t>
+  </si>
+  <si>
+    <t>dangerZoneTriviaResult1</t>
+  </si>
+  <si>
+    <t>dangerZoneTriviaResult2</t>
+  </si>
+  <si>
+    <t>dangerZoneTriviaResult3</t>
+  </si>
+  <si>
+    <t>dangerZoneTriviaResult4</t>
+  </si>
+  <si>
+    <t>dangerZoneTriviaResult5</t>
+  </si>
+  <si>
+    <t>A good way to quickly cool down a large amount of food is to divide it up to smaller portions.</t>
+  </si>
+  <si>
+    <t>Make sure not to take more than two hours to reheat food. Once the temperature reached 165° F, it should be ready.</t>
+  </si>
+  <si>
+    <t>Remember that hot food must retain its temperature above the Danger Zone (135° F). Discard hot food that has been sitting below 135° F for more than 2 hours!</t>
+  </si>
+  <si>
+    <t>Remember that cold food must retain its temperature below the Danger Zone (41° F). Discard any cold food that reaches above 70° F!</t>
+  </si>
+  <si>
+    <t>Remember that cold food may be held without refrigeration for up to 6 hours, starting from the time it was brought out.</t>
+  </si>
+  <si>
+    <t>A server was requested to check on the yogurt batch being served at the yogurt bar. After checking the temperature, it reads 72° F. Looking at the time it was brought out, it's been several hours.</t>
   </si>
 </sst>
 </file>
@@ -1288,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D156"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,15 +1365,15 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B4" t="s">
         <v>297</v>
-      </c>
-      <c r="B4" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1388,10 +1418,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" t="s">
         <v>289</v>
-      </c>
-      <c r="B10" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,26 +1450,26 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B14" t="s">
         <v>291</v>
-      </c>
-      <c r="B14" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B15" t="s">
         <v>293</v>
-      </c>
-      <c r="B15" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>294</v>
+      </c>
+      <c r="B16" t="s">
         <v>295</v>
-      </c>
-      <c r="B16" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1965,71 +1995,71 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>139</v>
+        <v>310</v>
       </c>
       <c r="B78" t="s">
-        <v>140</v>
+        <v>315</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B79" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B80" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B81" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B82" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>151</v>
+        <v>311</v>
       </c>
       <c r="B83" t="s">
-        <v>152</v>
+        <v>316</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B84" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B85" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B86" t="s">
         <v>157</v>
@@ -2037,592 +2067,632 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>159</v>
+        <v>312</v>
       </c>
       <c r="B87" t="s">
-        <v>160</v>
+        <v>317</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B89" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B90" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B91" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>15</v>
+        <v>313</v>
       </c>
       <c r="B92" t="s">
-        <v>300</v>
+        <v>319</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>16</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>301</v>
+        <v>166</v>
+      </c>
+      <c r="B93" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B94" t="s">
-        <v>302</v>
+        <v>168</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B95" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>174</v>
+        <v>314</v>
       </c>
       <c r="B96" t="s">
-        <v>175</v>
+        <v>318</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>176</v>
+        <v>15</v>
       </c>
       <c r="B97" t="s">
-        <v>177</v>
+        <v>299</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>179</v>
-      </c>
-      <c r="B98" t="s">
-        <v>304</v>
+        <v>16</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="B99" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B100" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B101" t="s">
-        <v>305</v>
-      </c>
-      <c r="C101">
-        <v>6</v>
+        <v>174</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B102" t="s">
-        <v>306</v>
-      </c>
-      <c r="C102">
-        <v>5</v>
+        <v>176</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B103" t="s">
-        <v>185</v>
-      </c>
-      <c r="C103">
-        <v>5</v>
+        <v>303</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B104" t="s">
-        <v>307</v>
-      </c>
-      <c r="C104">
-        <v>5</v>
+        <v>302</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B105" t="s">
-        <v>308</v>
+        <v>180</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B106" t="s">
-        <v>309</v>
+        <v>304</v>
+      </c>
+      <c r="C106">
+        <v>6</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B107" t="s">
-        <v>190</v>
+        <v>305</v>
+      </c>
+      <c r="C107">
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B108" t="s">
-        <v>193</v>
+        <v>184</v>
+      </c>
+      <c r="C108">
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B109" t="s">
-        <v>195</v>
+        <v>306</v>
+      </c>
+      <c r="C109">
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B110" t="s">
-        <v>197</v>
+        <v>307</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B111" t="s">
-        <v>199</v>
+        <v>308</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B112" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B113" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B114" t="s">
-        <v>310</v>
+        <v>194</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B115" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B116" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B117" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B118" t="s">
-        <v>212</v>
-      </c>
-      <c r="C118">
-        <v>1.5</v>
+        <v>202</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B119" t="s">
-        <v>214</v>
-      </c>
-      <c r="C119">
-        <v>8</v>
+        <v>309</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B120" t="s">
-        <v>217</v>
-      </c>
-      <c r="C120">
-        <v>2</v>
+        <v>205</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B121" t="s">
-        <v>218</v>
-      </c>
-      <c r="C121">
-        <v>8</v>
+        <v>207</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B122" t="s">
-        <v>221</v>
-      </c>
-      <c r="C122">
-        <v>1</v>
+        <v>209</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B123" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C123">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B124" t="s">
-        <v>224</v>
+        <v>213</v>
+      </c>
+      <c r="C124">
+        <v>8</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B125" t="s">
-        <v>227</v>
+        <v>216</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B126" t="s">
-        <v>228</v>
+        <v>217</v>
+      </c>
+      <c r="C126">
+        <v>8</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="B127" t="s">
-        <v>231</v>
+        <v>220</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="B128" t="s">
-        <v>232</v>
+        <v>221</v>
+      </c>
+      <c r="C128">
+        <v>8</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="B129" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="B130" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="B131" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B132" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="B133" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="B134" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B135" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B136" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="B137" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B138" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="B139" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B140" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B141" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="B142" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="B143" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="B144" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="B145" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>267</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>268</v>
+        <v>255</v>
+      </c>
+      <c r="B146" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="B147" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="B148" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="B149" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>274</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
+      </c>
+      <c r="B150" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B152" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>271</v>
+      </c>
+      <c r="B153" t="s">
         <v>277</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="B154" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>284</v>
-      </c>
-      <c r="B155" t="s">
-        <v>287</v>
+        <v>273</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>274</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>275</v>
+      </c>
+      <c r="B157" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>276</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>282</v>
+      </c>
+      <c r="B159" t="s">
         <v>285</v>
       </c>
-      <c r="B156" t="s">
-        <v>288</v>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>283</v>
+      </c>
+      <c r="B160" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>284</v>
+      </c>
+      <c r="B161" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>